<commit_message>
finished pre-data analysis pipeline, finalized MTurk paradigm
</commit_message>
<xml_diff>
--- a/data/FYP_data_children.xlsx
+++ b/data/FYP_data_children.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marianna\Desktop\Dropbox\Stanford\projects\FYP structural blocking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF4A382-BB50-42C1-819B-211F33F04F70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FAFC9E-FF8A-4B22-A74D-754ABFF04DD4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="1040" windowWidth="13970" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="1540" windowWidth="13560" windowHeight="9190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilot" sheetId="1" r:id="rId1"/>
     <sheet name="conditions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="60">
   <si>
     <t>gender</t>
   </si>
@@ -49,12 +49,6 @@
     <t>check_game</t>
   </si>
   <si>
-    <t>check_bucket_boy_1</t>
-  </si>
-  <si>
-    <t>check_bucket_boy_2</t>
-  </si>
-  <si>
     <t>context</t>
   </si>
   <si>
@@ -73,12 +67,6 @@
     <t>structural</t>
   </si>
   <si>
-    <t>check_bucket_girl_1</t>
-  </si>
-  <si>
-    <t>check_bucket_girl_2</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -130,34 +118,103 @@
     <t>innateness_switch</t>
   </si>
   <si>
-    <t>inductivePoten_expl</t>
-  </si>
-  <si>
-    <t>innateness_switch_expl</t>
-  </si>
-  <si>
-    <t>check_sample_boy_expl</t>
-  </si>
-  <si>
     <t>normative_group</t>
   </si>
   <si>
-    <t>normative_group_expl</t>
-  </si>
-  <si>
     <t>interference</t>
   </si>
   <si>
     <t>insuff_lang</t>
   </si>
   <si>
-    <t>check_sample_girl_expl</t>
-  </si>
-  <si>
-    <t>fc_expl_indiv_size</t>
-  </si>
-  <si>
-    <t>fc_expl_indiv_size_expl</t>
+    <t>Bing</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>ba1051</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>ba880</t>
+  </si>
+  <si>
+    <t>ba1047</t>
+  </si>
+  <si>
+    <t>ba894</t>
+  </si>
+  <si>
+    <t>ba875</t>
+  </si>
+  <si>
+    <t>bb254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ba1048 </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>FYP_20170417_01</t>
+  </si>
+  <si>
+    <t>FYP_20170417_02</t>
+  </si>
+  <si>
+    <t>FYP_20170417_03</t>
+  </si>
+  <si>
+    <t>FYP_20170419_01</t>
+  </si>
+  <si>
+    <t>FYP_20170419_02</t>
+  </si>
+  <si>
+    <t>FYP_20170419_03</t>
+  </si>
+  <si>
+    <t>FYP_20170419_04</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>FYP_20170420_01</t>
+  </si>
+  <si>
+    <t>FYP_20170420_02</t>
+  </si>
+  <si>
+    <t>FYP_20170420_03</t>
+  </si>
+  <si>
+    <t>FYP_20170420_04</t>
+  </si>
+  <si>
+    <t>FYP_20170420_05</t>
+  </si>
+  <si>
+    <t>FYP_20170420_06</t>
+  </si>
+  <si>
+    <t>witnessed her brother's answers to a different condition</t>
+  </si>
+  <si>
+    <t>check_bucket_boy</t>
+  </si>
+  <si>
+    <t>check_bucket_girl</t>
+  </si>
+  <si>
+    <t>fc_expl_indiv</t>
   </si>
 </sst>
 </file>
@@ -192,10 +249,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -314,12 +372,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -696,11 +755,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -714,232 +773,684 @@
     <col min="7" max="7" width="11.81640625" customWidth="1"/>
     <col min="8" max="8" width="10.36328125" customWidth="1"/>
     <col min="9" max="12" width="10" customWidth="1"/>
-    <col min="14" max="14" width="6.81640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="6.81640625" style="3" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="37" width="17.6328125" customWidth="1"/>
+    <col min="16" max="29" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
-        <v>36</v>
-      </c>
       <c r="L1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="O1" t="s">
         <v>3</v>
       </c>
       <c r="P1" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="Q1" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="R1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" t="s">
-        <v>13</v>
-      </c>
       <c r="T1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43572</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="V1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="3">
+        <v>5.5479452054794525</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43572</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="F3">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="3">
+        <v>5.2164383561643834</v>
+      </c>
+      <c r="O3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43572</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="3">
+        <v>5.0136986301369859</v>
+      </c>
+      <c r="O4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43574</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
       <c r="F5">
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="3">
+        <v>5.2082191780821914</v>
+      </c>
+      <c r="O5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43574</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="3">
+        <v>5.3260273972602743</v>
+      </c>
+      <c r="O6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43574</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="3">
+        <v>5.2767123287671236</v>
+      </c>
+      <c r="O7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43574</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="3">
+        <v>5.0986301369863014</v>
+      </c>
+      <c r="O8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43575</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43575</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43575</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
+      <c r="C12" s="2">
+        <v>43575</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43575</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
+        <v>43575</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+      <c r="X14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -955,205 +1466,208 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <f>COUNTIFS(pilot!$G:$G, B2, pilot!$H:$H, C2, pilot!$I:$I, D2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <f>COUNTIFS(pilot!$F:$F, A2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <f>COUNTIFS(pilot!$G:$G, B3, pilot!$H:$H, C3, pilot!$I:$I, D3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <f>COUNTIFS(pilot!$F:$F, A3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <f>COUNTIFS(pilot!$G:$G, B4, pilot!$H:$H, C4, pilot!$I:$I, D4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <f>COUNTIFS(pilot!$F:$F, A4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <f>COUNTIFS(pilot!$G:$G, B5, pilot!$H:$H, C5, pilot!$I:$I, D5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <f>COUNTIFS(pilot!$F:$F, A5)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <f>COUNTIFS(pilot!$G:$G, B6, pilot!$H:$H, C6, pilot!$I:$I, D6)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <f>COUNTIFS(pilot!$F:$F, A6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <f>COUNTIFS(pilot!$G:$G, B7, pilot!$H:$H, C7, pilot!$I:$I, D7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <f>COUNTIFS(pilot!$F:$F, A7)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <f>COUNTIFS(pilot!$G:$G, B8, pilot!$H:$H, C8, pilot!$I:$I, D8)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <f>COUNTIFS(pilot!$F:$F, A8)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <f>COUNTIFS(pilot!$G:$G, B9, pilot!$H:$H, C9, pilot!$I:$I, D9)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f>COUNTIFS(pilot!$F:$F, A9)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FYP brownbag talk, additional data collection
</commit_message>
<xml_diff>
--- a/data/FYP_data_children.xlsx
+++ b/data/FYP_data_children.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marianna\Desktop\Dropbox\Stanford\projects\FYP structural blocking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FC459C-5198-47C3-9F10-C052AF941415}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3DE491-78EE-4019-86B5-9AD4D20BEDCC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4030" yWindow="920" windowWidth="13560" windowHeight="9190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-260" yWindow="840" windowWidth="13560" windowHeight="9190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="145">
   <si>
     <t>gender</t>
   </si>
@@ -401,6 +401,75 @@
   </si>
   <si>
     <t>-&gt; Green-Ball</t>
+  </si>
+  <si>
+    <t>FYP_20190515_01</t>
+  </si>
+  <si>
+    <t>ba1102</t>
+  </si>
+  <si>
+    <t>ba1109</t>
+  </si>
+  <si>
+    <t>ba887</t>
+  </si>
+  <si>
+    <t>FYP_20190517_01</t>
+  </si>
+  <si>
+    <t>FYP_20190517_02</t>
+  </si>
+  <si>
+    <t>ba1184</t>
+  </si>
+  <si>
+    <t>ba963</t>
+  </si>
+  <si>
+    <t>FYP_20190520_01</t>
+  </si>
+  <si>
+    <t>FYP_20190520_02</t>
+  </si>
+  <si>
+    <t>Because she likes playing Yellow-Ball</t>
+  </si>
+  <si>
+    <t>FYP_20190519_01</t>
+  </si>
+  <si>
+    <t>FYP_20190519_02</t>
+  </si>
+  <si>
+    <t>FYP_20190519_03</t>
+  </si>
+  <si>
+    <t>FYP_20190519_04</t>
+  </si>
+  <si>
+    <t>FYP_20190519_05</t>
+  </si>
+  <si>
+    <t>FYP_20190519_06</t>
+  </si>
+  <si>
+    <t>FYP_20190519_07</t>
+  </si>
+  <si>
+    <t>FYP_20190519_08</t>
+  </si>
+  <si>
+    <t>-&gt; The green bucket is bigger</t>
+  </si>
+  <si>
+    <t>inductivePoten: "Green-Ball because she's a girl"</t>
+  </si>
+  <si>
+    <t>inductivePoten: "For sure Green-Ball because she's new and she doesn't know that much about them"</t>
+  </si>
+  <si>
+    <t>check_game: "The girls must play with the Yellow-Ball, and the boys must play with the Green-Ball"</t>
   </si>
 </sst>
 </file>
@@ -584,7 +653,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -607,7 +676,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -987,11 +1055,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z54" sqref="Z54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1191,7 +1259,7 @@
         <v>5.2164383561643834</v>
       </c>
       <c r="G3" s="18">
-        <f t="shared" ref="G3:G40" si="0">FLOOR(F3, 1)</f>
+        <f t="shared" ref="G3:G54" si="0">FLOOR(F3, 1)</f>
         <v>5</v>
       </c>
       <c r="H3" s="15" t="s">
@@ -1614,7 +1682,7 @@
       <c r="Q8" t="s">
         <v>41</v>
       </c>
-      <c r="R8" s="24" t="s">
+      <c r="R8" s="23" t="s">
         <v>107</v>
       </c>
       <c r="S8" t="s">
@@ -2021,29 +2089,29 @@
       <c r="C14" s="20">
         <v>43575</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="24" t="s">
         <v>42</v>
       </c>
       <c r="F14" s="21">
         <v>6.8520547945205479</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="15">
         <v>3</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="M14" s="19" t="s">
@@ -2502,7 +2570,7 @@
       <c r="R20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="S20" s="23" t="s">
+      <c r="S20" s="22" t="s">
         <v>100</v>
       </c>
       <c r="T20" s="11" t="s">
@@ -2577,7 +2645,7 @@
       <c r="R21" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="S21" s="23" t="s">
+      <c r="S21" s="22" t="s">
         <v>100</v>
       </c>
       <c r="T21" s="11" t="s">
@@ -2652,7 +2720,7 @@
       <c r="R22" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="S22" s="23" t="s">
+      <c r="S22" s="22" t="s">
         <v>111</v>
       </c>
       <c r="T22" s="11" t="s">
@@ -3024,10 +3092,10 @@
       <c r="Q27" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="R27" s="23" t="s">
+      <c r="R27" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="S27" s="23" t="s">
+      <c r="S27" s="22" t="s">
         <v>107</v>
       </c>
       <c r="T27" s="11" t="s">
@@ -3065,23 +3133,23 @@
       <c r="F28" s="21">
         <v>6.043835616438356</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="15">
         <v>2</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="J28" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L28" s="19" t="s">
+      <c r="L28" s="15" t="s">
         <v>7</v>
       </c>
       <c r="M28" s="19" t="s">
@@ -3113,23 +3181,23 @@
       <c r="F29" s="21">
         <v>6.043835616438356</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I29" s="19">
+      <c r="I29" s="15">
         <v>8</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="L29" s="19" t="s">
+      <c r="L29" s="15" t="s">
         <v>7</v>
       </c>
       <c r="M29" s="19" t="s">
@@ -3311,23 +3379,23 @@
       <c r="F32" s="21">
         <v>5.2657534246575342</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="19">
-        <v>6</v>
-      </c>
-      <c r="J32" s="19" t="s">
+      <c r="I32" s="15">
+        <v>6</v>
+      </c>
+      <c r="J32" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="19" t="s">
+      <c r="L32" s="15" t="s">
         <v>7</v>
       </c>
       <c r="M32" s="19" t="s">
@@ -3343,7 +3411,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>88</v>
       </c>
@@ -3418,7 +3486,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>87</v>
       </c>
@@ -3493,7 +3561,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>91</v>
       </c>
@@ -3568,7 +3636,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>92</v>
       </c>
@@ -3643,7 +3711,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>105</v>
       </c>
@@ -3721,7 +3789,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>106</v>
       </c>
@@ -3799,7 +3867,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>115</v>
       </c>
@@ -3877,7 +3945,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>116</v>
       </c>
@@ -3953,7 +4021,7 @@
       </c>
       <c r="Y40" s="11"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>117</v>
       </c>
@@ -3973,6 +4041,7 @@
         <v>5.0328767123287674</v>
       </c>
       <c r="G41" s="18">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H41" s="15" t="s">
@@ -4005,13 +4074,13 @@
       <c r="Q41" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="R41" s="23" t="s">
+      <c r="R41" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="S41" s="23" t="s">
+      <c r="S41" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="T41" s="23" t="s">
+      <c r="T41" s="22" t="s">
         <v>121</v>
       </c>
       <c r="U41" s="11" t="s">
@@ -4030,12 +4099,32 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A42" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="11">
+        <v>41</v>
+      </c>
+      <c r="C42" s="12">
+        <v>43600</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F42" s="14">
+        <v>5.5890410958904111</v>
+      </c>
+      <c r="G42" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="I42" s="15">
         <v>6</v>
       </c>
@@ -4048,24 +4137,72 @@
       <c r="L42" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="V42" s="11"/>
-      <c r="W42" s="11"/>
-      <c r="X42" s="11"/>
-      <c r="Y42" s="11"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
+      <c r="M42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q42" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R42" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="S42" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="T42" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="U42" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="V42" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="W42" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="X42" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y42" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A43" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="11">
+        <v>42</v>
+      </c>
+      <c r="C43" s="12">
+        <v>43602</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="14">
+        <v>5.2136986301369861</v>
+      </c>
+      <c r="G43" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>32</v>
+      </c>
       <c r="I43" s="15">
         <v>1</v>
       </c>
@@ -4078,19 +4215,75 @@
       <c r="L43" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="11"/>
-      <c r="V43" s="11"/>
-      <c r="W43" s="11"/>
-      <c r="X43" s="11"/>
-      <c r="Y43" s="11"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="M43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q43" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R43" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="S43" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="T43" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="U43" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="V43" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="W43" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="X43" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y43" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z43" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44" s="12">
+        <v>43602</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="14">
+        <v>5.0493150684931507</v>
+      </c>
+      <c r="G44" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>32</v>
+      </c>
       <c r="I44" s="15">
         <v>5</v>
       </c>
@@ -4103,19 +4296,69 @@
       <c r="L44" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-      <c r="S44" s="11"/>
-      <c r="V44" s="11"/>
-      <c r="W44" s="11"/>
-      <c r="X44" s="11"/>
-      <c r="Y44" s="11"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="M44" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N44" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O44" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P44" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q44" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R44" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="S44" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="T44" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="U44" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="V44" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="W44" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="X44" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y44" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" s="2">
+        <v>43604</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" s="14">
+        <v>5.6767123287671231</v>
+      </c>
+      <c r="G45" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="I45" s="15">
         <v>7</v>
       </c>
@@ -4128,19 +4371,69 @@
       <c r="L45" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
-      <c r="V45" s="11"/>
-      <c r="W45" s="11"/>
-      <c r="X45" s="11"/>
-      <c r="Y45" s="11"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="M45" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N45" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O45" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P45" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q45" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R45" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="S45" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="T45" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="U45" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="V45" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="W45" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="X45" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y45" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A46" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" s="2">
+        <v>43604</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="14">
+        <v>5.8794520547945206</v>
+      </c>
+      <c r="G46" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="I46" s="15">
         <v>8</v>
       </c>
@@ -4153,23 +4446,671 @@
       <c r="L46" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-      <c r="S46" s="11"/>
-      <c r="V46" s="11"/>
-      <c r="W46" s="11"/>
-      <c r="X46" s="11"/>
-      <c r="Y46" s="11"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V47" s="11"/>
-      <c r="W47" s="11"/>
-      <c r="X47" s="11"/>
-      <c r="Y47" s="11"/>
+      <c r="M46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q46" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R46" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="S46" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="T46" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="U46" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="V46" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="W46" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="X46" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y46" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="7">
+        <v>46</v>
+      </c>
+      <c r="C47" s="8">
+        <v>43604</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="10">
+        <v>5.934246575342466</v>
+      </c>
+      <c r="G47" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I47" s="15">
+        <v>4</v>
+      </c>
+      <c r="J47" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K47" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L47" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q47" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="T47" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="W47" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="X47" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y47" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="7">
+        <v>47</v>
+      </c>
+      <c r="C48" s="8">
+        <v>43604</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="10">
+        <v>5.9013698630136986</v>
+      </c>
+      <c r="G48" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I48" s="15">
+        <v>5</v>
+      </c>
+      <c r="J48" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L48" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P48" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q48" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R48" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="S48" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="T48" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="U48" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="V48" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="W48" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="X48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y48" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z48" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" s="7">
+        <v>48</v>
+      </c>
+      <c r="C49" s="8">
+        <v>43604</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F49" s="10">
+        <v>5.86027397260274</v>
+      </c>
+      <c r="G49" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I49" s="15">
+        <v>2</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K49" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L49" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P49" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q49" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R49" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="T49" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="U49" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="V49" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="W49" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="X49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y49" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" s="7">
+        <v>49</v>
+      </c>
+      <c r="C50" s="8">
+        <v>43604</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F50" s="10">
+        <v>5.8191780821917805</v>
+      </c>
+      <c r="G50" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I50" s="15">
+        <v>7</v>
+      </c>
+      <c r="J50" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K50" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L50" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q50" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R50" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="S50" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="T50" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="U50" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="V50" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="W50" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="X50" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y50" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="7">
+        <v>50</v>
+      </c>
+      <c r="C51" s="8">
+        <v>43604</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" s="10">
+        <v>5.3150684931506849</v>
+      </c>
+      <c r="G51" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" s="15">
+        <v>8</v>
+      </c>
+      <c r="J51" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K51" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L51" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q51" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R51" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="T51" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="U51" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="W51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="X51" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y51" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" s="7">
+        <v>51</v>
+      </c>
+      <c r="C52" s="8">
+        <v>43604</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F52" s="10">
+        <v>5.3150684931506849</v>
+      </c>
+      <c r="G52" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I52" s="15">
+        <v>1</v>
+      </c>
+      <c r="J52" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K52" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L52" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q52" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R52" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="T52" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="U52" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="V52" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="W52" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="X52" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y52" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="11">
+        <v>52</v>
+      </c>
+      <c r="C53" s="12">
+        <v>43605</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F53" s="14">
+        <v>5.0191780821917806</v>
+      </c>
+      <c r="G53" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" s="15">
+        <v>2</v>
+      </c>
+      <c r="J53" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K53" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L53" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N53" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O53" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P53" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q53" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R53" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="S53" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="T53" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="U53" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="V53" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="W53" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="X53" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y53" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z53" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="11">
+        <v>53</v>
+      </c>
+      <c r="C54" s="12">
+        <v>43605</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F54" s="14">
+        <v>5.2876712328767121</v>
+      </c>
+      <c r="G54" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I54" s="15">
+        <v>6</v>
+      </c>
+      <c r="J54" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K54" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L54" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M54" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N54" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O54" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P54" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q54" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R54" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="S54" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="T54" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="U54" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="V54" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="W54" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="X54" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y54" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="I55" s="15">
+        <v>3</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K55" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L55" s="15" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4186,8 +5127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4264,7 +5205,7 @@
       </c>
       <c r="S2" s="6">
         <f>SUM(E1:E20, N1:N20)</f>
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -4282,11 +5223,11 @@
       </c>
       <c r="E3">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$J:$J, B3, data!$K:$K, C3, data!$L:$L, D3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$I:$I, A3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -4333,11 +5274,11 @@
       </c>
       <c r="E4">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$J:$J, B4, data!$K:$K, C4, data!$L:$L, D4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$I:$I, A4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4">
         <v>6</v>
@@ -4437,11 +5378,11 @@
       </c>
       <c r="E6">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$J:$J, B6, data!$K:$K, C6, data!$L:$L, D6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$I:$I, A6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>6</v>
@@ -4486,11 +5427,11 @@
       </c>
       <c r="E7">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$J:$J, B7, data!$K:$K, C7, data!$L:$L, D7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$I:$I, A7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -4534,11 +5475,11 @@
       </c>
       <c r="E8">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$J:$J, B8, data!$K:$K, C8, data!$L:$L, D8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$I:$I, A8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>6</v>
@@ -4582,11 +5523,11 @@
       </c>
       <c r="E9">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$J:$J, B9, data!$K:$K, C9, data!$L:$L, D9)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$I:$I, A9)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9">
         <v>6</v>
@@ -4630,11 +5571,11 @@
       </c>
       <c r="E10">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$J:$J, B10, data!$K:$K, C10, data!$L:$L, D10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$2, data!$I:$I, A10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>6</v>
@@ -4773,11 +5714,11 @@
       </c>
       <c r="E14">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$J:$J, B14, data!$K:$K, C14, data!$L:$L, D14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$I:$I, A14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>6</v>
@@ -4920,11 +5861,11 @@
       </c>
       <c r="E17">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$J:$J, B17, data!$K:$K, C17, data!$L:$L, D17)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F17">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$I:$I, A17)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17">
         <v>6</v>
@@ -4968,11 +5909,11 @@
       </c>
       <c r="E18">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$J:$J, B18, data!$K:$K, C18, data!$L:$L, D18)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F18">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$I:$I, A18)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G18">
         <v>-1</v>
@@ -5019,11 +5960,11 @@
       </c>
       <c r="E19">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$J:$J, B19, data!$K:$K, C19, data!$L:$L, D19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$I:$I, A19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>6</v>
@@ -5067,11 +6008,11 @@
       </c>
       <c r="E20">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$J:$J, B20, data!$K:$K, C20, data!$L:$L, D20)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20">
         <f>COUNTIFS(data!$G:$G, $A$1, data!$H:$H, $A$12, data!$I:$I, A20)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>6</v>

</xml_diff>

<commit_message>
FYP report submit, adult replication run
</commit_message>
<xml_diff>
--- a/data/FYP_data_children.xlsx
+++ b/data/FYP_data_children.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marianna\Desktop\Dropbox\Stanford\projects\FYP structural blocking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3DE491-78EE-4019-86B5-9AD4D20BEDCC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B6F5DC-E7E1-474E-96DB-042028CE5025}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-260" yWindow="840" windowWidth="13560" windowHeight="9190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="13560" windowHeight="9190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1057,9 +1057,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z54" sqref="Z54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5128,7 +5128,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>